<commit_message>
cadastro completo, falta verificação
</commit_message>
<xml_diff>
--- a/Cronograma_TCC.xlsx
+++ b/Cronograma_TCC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Documentos\Coisas do Pedro Lindo\GitHub\tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB4E210-8B95-4ABC-AC0D-19D5A5E0ED51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F840D2-E917-461B-BAC4-6B923C857A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0B942D0F-70D3-4C87-A812-C8EDC081A5CA}"/>
   </bookViews>
@@ -99,12 +99,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -138,6 +144,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE508E2-D9D8-4C42-B559-08CCA060AF0F}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +483,7 @@
       <c r="A2" s="2">
         <v>44774</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -485,7 +494,7 @@
       <c r="A3" s="2">
         <v>44774</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -493,7 +502,7 @@
       <c r="A4" s="2">
         <v>44781</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
iniciando a inscrição do usuário
</commit_message>
<xml_diff>
--- a/Cronograma_TCC.xlsx
+++ b/Cronograma_TCC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Documentos\Coisas do Pedro Lindo\GitHub\tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F840D2-E917-461B-BAC4-6B923C857A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FAAFA7-3CE1-4BD9-BFDE-C318BBF4B9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0B942D0F-70D3-4C87-A812-C8EDC081A5CA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>28/11/2022
 29/11/2022</t>
@@ -52,12 +52,6 @@
   <si>
     <t>Cadastro do profissional
 (ver documentos e regras necessárias)</t>
-  </si>
-  <si>
-    <t>Publicações/perfis
-Formulário de inscrição em eventos
-Formulário de requisição
-de voluntários</t>
   </si>
   <si>
     <t>acessibilidade no app</t>
@@ -84,16 +78,44 @@
   </si>
   <si>
     <t>Subir servidores para a Internet e comprar um domínio (P.C.)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Publicações/perfis
+Formulário de inscrição em eventos
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Formulário de requisição
+de voluntários</t>
+    </r>
+  </si>
+  <si>
+    <t>O Voluntário ainda não foi implementado por causa de alguns BUGs em relação ao tabnavigator do mesmo.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -464,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE508E2-D9D8-4C42-B559-08CCA060AF0F}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +509,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -497,6 +519,7 @@
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -505,13 +528,17 @@
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44788</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -521,6 +548,7 @@
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -529,6 +557,7 @@
       <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -537,6 +566,7 @@
       <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -545,82 +575,94 @@
       <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44823</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44830</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44837</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44844</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>10</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44851</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44858</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>14</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44865</v>
       </c>
       <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="1:2" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44872</v>
       </c>
       <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44879</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" s="1" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>44886</v>
       </c>
       <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:2" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="D20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
terminando detalhes da alteração de perfil e perfil da ong
</commit_message>
<xml_diff>
--- a/Cronograma_TCC.xlsx
+++ b/Cronograma_TCC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Documentos\Coisas do Pedro Lindo\GitHub\tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A6DE56-5D29-4847-8D73-9E8D339AB6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828B58ED-D8A0-4327-8C32-0529DDF7E92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0B942D0F-70D3-4C87-A812-C8EDC081A5CA}"/>
   </bookViews>
@@ -26,10 +26,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t>28/11/2022
-29/11/2022</t>
-  </si>
   <si>
     <t>Organização do projeto, instalação dos softwares necessários</t>
   </si>
@@ -112,6 +108,10 @@
   </si>
   <si>
     <t>Apresentação!!!</t>
+  </si>
+  <si>
+    <t>25/11/2022
+26/11/2022</t>
   </si>
 </sst>
 </file>
@@ -147,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,12 +166,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -185,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,9 +206,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -533,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE508E2-D9D8-4C42-B559-08CCA060AF0F}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,10 +545,10 @@
         <v>44774</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -565,7 +556,7 @@
         <v>44774</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4"/>
     </row>
@@ -574,7 +565,7 @@
         <v>44781</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -583,11 +574,11 @@
         <v>44788</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -595,10 +586,10 @@
         <v>44795</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -606,7 +597,7 @@
         <v>44802</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="4"/>
     </row>
@@ -615,7 +606,7 @@
         <v>44809</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -623,8 +614,8 @@
       <c r="A9" s="2">
         <v>44816</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>5</v>
+      <c r="B9" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="D9" s="4"/>
     </row>
@@ -633,7 +624,7 @@
         <v>44823</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="4"/>
     </row>
@@ -642,7 +633,7 @@
         <v>44830</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -651,7 +642,7 @@
         <v>44837</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="4"/>
     </row>
@@ -660,15 +651,15 @@
         <v>44844</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44851</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>10</v>
+      <c r="B14" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D14" s="4"/>
     </row>
@@ -677,7 +668,7 @@
         <v>44858</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="4"/>
     </row>
@@ -710,10 +701,10 @@
     </row>
     <row r="20" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="4"/>
     </row>

</xml_diff>

<commit_message>
BUGS CONSERTADOS: 1. Deletar um comentario nao causa mais erro no servidor 2. Inscrever-se em uma ONG nao causa mais erro no servidor 3. Desinscrever-se de um evento pela tela de inscricoes nao causa mais erro no servidor.
</commit_message>
<xml_diff>
--- a/Cronograma_TCC.xlsx
+++ b/Cronograma_TCC.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Documentos\Coisas do Pedro Lindo\GitHub\tcc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coisas do amorzaum s2\Github\tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828B58ED-D8A0-4327-8C32-0529DDF7E92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0B942D0F-70D3-4C87-A812-C8EDC081A5CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Organização do projeto, instalação dos softwares necessários</t>
   </si>
@@ -48,17 +47,6 @@
   <si>
     <t>Cadastro do profissional
 (ver documentos e regras necessárias)</t>
-  </si>
-  <si>
-    <t>acessibilidade no app</t>
-  </si>
-  <si>
-    <t>Regulação LGPD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sistema de compartilhamento de eventos por link do app
-QR code
-</t>
   </si>
   <si>
     <t>Sistema de gerar posters pro evento (PHP to PDF/PNG)</t>
@@ -71,9 +59,6 @@
   </si>
   <si>
     <t>Pegar dados dos eventos, compartilhamentos/likes</t>
-  </si>
-  <si>
-    <t>Subir servidores para a Internet e comprar um domínio (P.C.)</t>
   </si>
   <si>
     <t>Limpeza e melhoramento do código feito até agora</t>
@@ -117,7 +102,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -206,6 +191,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -521,26 +509,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE508E2-D9D8-4C42-B559-08CCA060AF0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44774</v>
       </c>
@@ -548,10 +536,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44774</v>
       </c>
@@ -560,7 +548,7 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44781</v>
       </c>
@@ -569,19 +557,19 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44788</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44795</v>
       </c>
@@ -589,10 +577,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44802</v>
       </c>
@@ -601,7 +589,7 @@
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44809</v>
       </c>
@@ -610,7 +598,7 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44816</v>
       </c>
@@ -619,92 +607,84 @@
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44823</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44830</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44837</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="B12" s="6"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44844</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44851</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="B14" s="10"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44858</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B15" s="5"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44865</v>
       </c>
       <c r="B16" s="6"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44872</v>
       </c>
       <c r="B17" s="6"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44879</v>
       </c>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>44886</v>
       </c>
       <c r="B19" s="6"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D20" s="4"/>
     </row>

</xml_diff>